<commit_message>
changing the database for rectifying errors
</commit_message>
<xml_diff>
--- a/data_insertion/parking details.xlsx
+++ b/data_insertion/parking details.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
@@ -9,13 +9,48 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>2018-06-03 06:00:00</t>
+  </si>
+  <si>
+    <t>2018-06-03 06:30:00</t>
+  </si>
+  <si>
+    <t>2018-06-03 07:00:00</t>
+  </si>
+  <si>
+    <t>2018-06-03 07:10:00</t>
+  </si>
+  <si>
+    <t>2018-06-03 07:40:00</t>
+  </si>
+  <si>
+    <t>2018-06-03 07:50:00</t>
+  </si>
+  <si>
+    <t>2018-06-03 08:30:00</t>
+  </si>
+  <si>
+    <t>2018-06-13 09:30:00</t>
+  </si>
+  <si>
+    <t>2018-06-13 10:00:00</t>
+  </si>
+  <si>
+    <t>2018-06-13 11:00:00</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -49,8 +84,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -144,6 +180,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -179,6 +232,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -331,12 +401,201 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="5" max="5" width="99.5703125" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>4</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="str">
+        <f>CONCATENATE("insert into [dbo].[parking] ([park ID],[vehicle id],[slot ID],[in time]) values(",A1,",",B1,",",C1,",'",D1,"')")</f>
+        <v>insert into [dbo].[parking] ([park ID],[vehicle id],[slot ID],[in time]) values(1,4,2,'2018-06-03 06:00:00')</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>65</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="str">
+        <f t="shared" ref="E2:E10" si="0">CONCATENATE("insert into [dbo].[parking] ([park ID],[vehicle id],[slot ID],[in time]) values(",A2,",",B2,",",C2,",'",D2,"')")</f>
+        <v>insert into [dbo].[parking] ([park ID],[vehicle id],[slot ID],[in time]) values(2,1,65,'2018-06-03 06:30:00')</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>45</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into [dbo].[parking] ([park ID],[vehicle id],[slot ID],[in time]) values(3,3,45,'2018-06-03 07:00:00')</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>87</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into [dbo].[parking] ([park ID],[vehicle id],[slot ID],[in time]) values(4,8,87,'2018-06-03 07:10:00')</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>112</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into [dbo].[parking] ([park ID],[vehicle id],[slot ID],[in time]) values(5,12,112,'2018-06-03 07:40:00')</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>17</v>
+      </c>
+      <c r="C6">
+        <v>118</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into [dbo].[parking] ([park ID],[vehicle id],[slot ID],[in time]) values(6,17,118,'2018-06-03 07:50:00')</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>194</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into [dbo].[parking] ([park ID],[vehicle id],[slot ID],[in time]) values(7,6,194,'2018-06-03 08:30:00')</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>19</v>
+      </c>
+      <c r="C8">
+        <v>154</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into [dbo].[parking] ([park ID],[vehicle id],[slot ID],[in time]) values(8,19,154,'2018-06-13 09:30:00')</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>100</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into [dbo].[parking] ([park ID],[vehicle id],[slot ID],[in time]) values(9,7,100,'2018-06-13 10:00:00')</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>11</v>
+      </c>
+      <c r="C10">
+        <v>34</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into [dbo].[parking] ([park ID],[vehicle id],[slot ID],[in time]) values(10,11,34,'2018-06-13 11:00:00')</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>